<commit_message>
add scripts and update readme
</commit_message>
<xml_diff>
--- a/Records.xlsx
+++ b/Records.xlsx
@@ -5,14 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Benchmark Sequences" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Benchmark_Sequences" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Rules" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="freiburg3_long_office_household" vbProcedure="false">'Benchmark Sequences'!$C$79</definedName>
+    <definedName function="false" hidden="false" name="freiburg3_long_office_household" vbProcedure="false">Benchmark_Sequences!$C$79</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="176">
   <si>
     <t xml:space="preserve">for properties motion_dynamics, environment_dynamics and revisit_frequency, we use low, medium and high, three levels to evaluate their properties, where we mark revisit_frequency of sequences that keep wandering in a small space as low. The difficulty level for each sequence is evaluated based on 1) existing assigned flags, 2) VO/SLAM results reported from ours and others and 3) manually evaluation.</t>
   </si>
@@ -41,13 +41,13 @@
     <t xml:space="preserve">Platform</t>
   </si>
   <si>
-    <t xml:space="preserve">In-/Outdoor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duration (s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motion_Dyn (DoF)</t>
+    <t xml:space="preserve">Scene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motion_Dyn</t>
   </si>
   <si>
     <t xml:space="preserve">Env_Dyn</t>
@@ -507,9 +507,6 @@
   </si>
   <si>
     <t xml:space="preserve">High/Long</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duration</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;2 mins</t>
@@ -848,19 +845,20 @@
   </sheetPr>
   <dimension ref="A1:M65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.3724489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="40.219387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="4" style="1" width="22.734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.4234693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="46.4897959183674"/>
+    <col collapsed="false" hidden="false" max="10" min="4" style="1" width="26.2244897959184"/>
     <col collapsed="false" hidden="true" max="11" min="11" style="3" width="0"/>
     <col collapsed="false" hidden="true" max="13" min="12" style="4" width="0"/>
-    <col collapsed="false" hidden="false" max="1023" min="14" style="5" width="18"/>
+    <col collapsed="false" hidden="false" max="1023" min="14" style="5" width="20.780612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.66326530612245"/>
   </cols>
   <sheetData>
     <row r="1" s="9" customFormat="true" ht="65.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4779,15 +4777,15 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2040816326531"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="44.5357142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="12.3367346938776"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.9795918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="51.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="14.1938775510204"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="34.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4804,58 +4802,58 @@
     </row>
     <row r="2" customFormat="false" ht="42.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="C2" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="D2" s="16" t="s">
         <v>163</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="42.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="C3" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="D3" s="16" t="s">
         <v>167</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="90.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="C4" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>171</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="90.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="C5" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="D5" s="16" t="s">
         <v>175</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>